<commit_message>
working, graphs of use freq would be nice
</commit_message>
<xml_diff>
--- a/Pharma HalfLive.xlsx
+++ b/Pharma HalfLive.xlsx
@@ -24,21 +24,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date taken</t>
   </si>
   <si>
-    <t>Date Now</t>
-  </si>
-  <si>
-    <t>Difference</t>
-  </si>
-  <si>
-    <t>6/22/2020  4:314:00 PM</t>
-  </si>
-  <si>
-    <t>TIMEVALUE("8:30 PM") - TIMEVALUE("6:40 AM")</t>
+    <t>lamba/time decay constant</t>
+  </si>
+  <si>
+    <t>for primary</t>
+  </si>
+  <si>
+    <t>for metabolite</t>
+  </si>
+  <si>
+    <t>half life</t>
+  </si>
+  <si>
+    <t>Initial (mg)</t>
+  </si>
+  <si>
+    <t>Final Primary (mg)</t>
+  </si>
+  <si>
+    <t>Final Metabolite (mg)</t>
+  </si>
+  <si>
+    <t>Current Time</t>
+  </si>
+  <si>
+    <t>Time Constant (hr)</t>
   </si>
 </sst>
 </file>
@@ -55,9 +70,9 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF454545"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,9 +98,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="18" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,67 +415,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
-    <col min="2" max="3" width="32.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>44003.676388888889</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <f ca="1">B2*EXP($I$3*E2*-1)</f>
+        <v>8.9924908886031222E-3</v>
+      </c>
+      <c r="D2">
+        <f ca="1">B2*EXP($I$4*E2*-1)</f>
+        <v>0.27763949637769614</v>
+      </c>
+      <c r="E2" s="4">
+        <f ca="1">($I$6-A2+($I$6&lt;A2))*24</f>
+        <v>30.789722222252749</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>44003.676388888889</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f ca="1">B3*EXP($I$3*E3*-1)</f>
+        <v>6.7443681664523421E-3</v>
+      </c>
+      <c r="D3">
+        <f ca="1">B3*EXP($I$4*E3*-1)</f>
+        <v>0.2082296222832721</v>
+      </c>
+      <c r="E3" s="4">
+        <f ca="1">($I$6-A3+($I$6&lt;A3))*24</f>
+        <v>30.789722222252749</v>
+      </c>
+      <c r="G3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="H3">
+        <v>3.5</v>
+      </c>
+      <c r="I3">
+        <f>(-LN(1/2))/H3</f>
+        <v>0.19804205158855578</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>44003.676388888889</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
-        <v>44004.688888888886</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4">
+        <f t="shared" ref="C4:C9" ca="1" si="0">B4*EXP($I$3*E4*-1)</f>
+        <v>6.7443681664523421E-3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D9" ca="1" si="1">B4*EXP($I$4*E4*-1)</f>
+        <v>0.2082296222832721</v>
+      </c>
+      <c r="E4" s="4">
+        <f ca="1">($I$6-A4+($I$6&lt;A4))*24</f>
+        <v>30.789722222252749</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <f>(-LN(1/2))/H4</f>
+        <v>8.6643397569993161E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44004.676388888889</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.78189233265459956</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6658369782661766</v>
+      </c>
+      <c r="E5" s="4">
+        <f ca="1">($I$6-A5+($I$6&lt;A5))*24</f>
+        <v>6.7897222222527489</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44004.676388888889</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3031538877576661</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.7763949637769607</v>
+      </c>
+      <c r="E6" s="4">
+        <f ca="1">($I$6-A6+($I$6&lt;A6))*24</f>
+        <v>6.7897222222527489</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1">
+        <f ca="1">NOW()</f>
+        <v>44004.959293981483</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44004.676388888889</v>
+      </c>
+      <c r="B7">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
-        <f ca="1">NOW()</f>
-        <v>44004.694246180552</v>
-      </c>
-      <c r="C3" s="3" t="e">
-        <f>TIMEVALUE((A2)) - (TIMEVALUE(B2))</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="e">
-        <f ca="1">B3-A2</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="e">
-        <f>INT(B2-A2) &amp; " days, " &amp; HOUR(B2-A2) &amp; " hours, " &amp; MINUTE(B2-A2) &amp; " minutes and " &amp; SECOND(B2-A2) &amp; " seconds"</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="4">
-        <f>TIME(HOUR(4),MINUTE(14),SECOND(0))</f>
-        <v>0</v>
-      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.0425231102061328</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.2211159710215687</v>
+      </c>
+      <c r="E7" s="4">
+        <f ca="1">($I$6-A7+($I$6&lt;A7))*24</f>
+        <v>6.7897222222527489</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44004.676388888889</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.78189233265459956</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6658369782661766</v>
+      </c>
+      <c r="E8" s="4">
+        <f ca="1">($I$6-A8+($I$6&lt;A8))*24</f>
+        <v>6.7897222222527489</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44004.676388888889</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.26063077755153319</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.55527899275539216</v>
+      </c>
+      <c r="E9" s="4">
+        <f ca="1">($I$6-A9+($I$6&lt;A9))*24</f>
+        <v>6.7897222222527489</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44004.676388888889</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <f ca="1">B10*EXP($I$3*E10*-1)</f>
+        <v>0.52126155510306638</v>
+      </c>
+      <c r="D10">
+        <f ca="1">B10*EXP($I$4*E10*-1)</f>
+        <v>1.1105579855107843</v>
+      </c>
+      <c r="E10" s="4">
+        <f ca="1">($I$6-A10+($I$6&lt;A10))*24</f>
+        <v>6.7897222222527489</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
may refractor to change needing reference to  direct cells for things like equalsNow to get time
</commit_message>
<xml_diff>
--- a/Pharma HalfLive.xlsx
+++ b/Pharma HalfLive.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date taken</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>Time Constant (hr)</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Metabolite</t>
+  </si>
+  <si>
+    <t>half lives past since</t>
   </si>
 </sst>
 </file>
@@ -95,12 +110,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,16 +431,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
@@ -433,7 +449,7 @@
     <col min="10" max="10" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,24 +466,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>44003.676388888889</v>
+        <v>44003.738888888889</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
       <c r="C2">
         <f ca="1">B2*EXP($I$3*E2*-1)</f>
-        <v>8.8760000859239001E-3</v>
+        <v>1.135333159651194E-2</v>
       </c>
       <c r="D2">
         <f ca="1">B2*EXP($I$4*E2*-1)</f>
-        <v>0.27606020928542863</v>
+        <v>0.30745049648677591</v>
       </c>
       <c r="E2" s="4">
-        <f t="shared" ref="E2:E10" ca="1" si="0">($I$6-A2+($I$6&lt;A2))*24</f>
-        <v>30.855561111064162</v>
+        <f ca="1">($I$6-A2+($I$6&lt;A2))*24</f>
+        <v>29.612591666635126</v>
+      </c>
+      <c r="F2">
+        <f ca="1">E2/$H$3</f>
+        <v>8.4607404761814653</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
@@ -476,24 +496,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>44003.676388888889</v>
+        <v>44003.75</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3">
         <f ca="1">B3*EXP($I$3*E3*-1)</f>
-        <v>6.6570000644429247E-3</v>
+        <v>8.9767722035911379E-3</v>
       </c>
       <c r="D3">
         <f ca="1">B3*EXP($I$4*E3*-1)</f>
-        <v>0.20704515696407147</v>
+        <v>0.23597760838943019</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ca="1" si="0"/>
-        <v>30.855561111064162</v>
+        <f t="shared" ref="E2:E10" ca="1" si="0">($I$6-A3+($I$6&lt;A3))*24</f>
+        <v>29.34592499997234</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F10" ca="1" si="1">E3/$H$3</f>
+        <v>8.3845499999920978</v>
       </c>
       <c r="G3" t="s">
         <v>2</v>
@@ -506,24 +530,28 @@
         <v>0.19804205158855578</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>44003.676388888889</v>
+        <v>44003.780555555553</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C9" ca="1" si="1">B4*EXP($I$3*E4*-1)</f>
-        <v>6.6570000644429247E-3</v>
+        <f t="shared" ref="C4:C9" ca="1" si="2">B4*EXP($I$3*E4*-1)</f>
+        <v>1.0379899677524704E-2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D9" ca="1" si="2">B4*EXP($I$4*E4*-1)</f>
-        <v>0.20704515696407147</v>
+        <f t="shared" ref="D4:D9" ca="1" si="3">B4*EXP($I$4*E4*-1)</f>
+        <v>0.25145785787168318</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>30.855561111064162</v>
+        <v>28.612591666693334</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.1750261904838091</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
@@ -535,115 +563,141 @@
         <f>(-LN(1/2))/H4</f>
         <v>8.6643397569993161E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>44004.676388888889</v>
+        <v>44004.169444444444</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.77176351889565553</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>6.5908254670214841E-2</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.6563612557125718</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.56450380442217141</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8555611110641621</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>19.279258333321195</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.5083595238060559</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>44004.676388888889</v>
+        <v>44004.17291666667</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.2862725314927592</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.11167499498128362</v>
       </c>
       <c r="D6">
-        <f t="shared" ca="1" si="2"/>
-        <v>2.7606020928542865</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.94765738615940487</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8555611110641621</v>
+        <v>19.195924999890849</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.4845499999688139</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="1">
         <f ca="1">NOW()</f>
-        <v>44004.962037268517</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44004.972746874999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>44004.676388888889</v>
+        <v>44004.196527777778</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.0290180251942074</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.9950303774108906E-2</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="2"/>
-        <v>2.208481674283429</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.79627722983449312</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8555611110641621</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18.629258333297912</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.3226452380851175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>44004.676388888889</v>
+        <v>44004.240972222222</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.77176351889565553</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.2595068359346874E-2</v>
       </c>
       <c r="D8">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.6563612557125718</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.65503256733250215</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8555611110641621</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>17.562591666646767</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.0178833333276476</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>44004.676388888889</v>
+        <v>44004.583333333336</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.25725450629855184</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.15709789059236889</v>
       </c>
       <c r="D9">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.55212041857085725</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.44496364560317636</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8555611110641621</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9.3459249999141321</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.6702642856897518</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44004.676388888889</v>
       </c>
@@ -652,18 +706,48 @@
       </c>
       <c r="C10">
         <f ca="1">B10*EXP($I$3*E10*-1)</f>
-        <v>0.51450901259710369</v>
+        <v>0.48897443784846156</v>
       </c>
       <c r="D10">
         <f ca="1">B10*EXP($I$4*E10*-1)</f>
-        <v>1.1042408371417145</v>
+        <v>1.0799211973254876</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8555611110641621</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>7.1125916666351259</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.032169047610036</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G11" s="5">
+        <f>SUM(B:B)</f>
+        <v>28</v>
+      </c>
+      <c r="H11">
+        <f ca="1">SUM(C:C)</f>
+        <v>1.0469109537034125</v>
+      </c>
+      <c r="I11">
+        <f ca="1">SUM(D:D)</f>
+        <v>5.283241793425125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E13" s="2"/>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
graph excel can't use minutes or hours, only months years for date
</commit_message>
<xml_diff>
--- a/Pharma HalfLive.xlsx
+++ b/Pharma HalfLive.xlsx
@@ -129,6 +129,943 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Initial</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (mg) vs Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.62893744531933504"/>
+          <c:y val="7.407407407407407E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy\ h:mm</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>44003.738888888889</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44003.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44003.780555555553</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44004.169444444444</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44004.17291666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44004.196527777778</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44004.240972222222</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44004.583333333336</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44004.676388888889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D9E-458A-8220-693EDD35AA0E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1750302655"/>
+        <c:axId val="1753491679"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1750302655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy\ h:mm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1753491679"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1753491679"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1750302655"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,8 +1367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,5 +1689,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>